<commit_message>
Reformatted grammar and added instrumental usage
</commit_message>
<xml_diff>
--- a/data/vocabulary.xlsx
+++ b/data/vocabulary.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christie/github/buddhavacana/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E089454-E850-0945-9D6A-0D854CFC7D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2019C3E-A95E-9946-B734-9AFF54299705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="21600" activeTab="2" xr2:uid="{29D2D6BB-F855-BC40-BB49-97E9609A8E50}"/>
   </bookViews>
   <sheets>
     <sheet name="Verbs" sheetId="1" r:id="rId1"/>
     <sheet name="Nouns" sheetId="2" r:id="rId2"/>
-    <sheet name="Pronouns" sheetId="5" r:id="rId3"/>
-    <sheet name="Adjectives" sheetId="4" r:id="rId4"/>
-    <sheet name="Indeclinables" sheetId="3" r:id="rId5"/>
+    <sheet name="Irregulars" sheetId="6" r:id="rId3"/>
+    <sheet name="Pronouns" sheetId="5" r:id="rId4"/>
+    <sheet name="Adjectives" sheetId="4" r:id="rId5"/>
+    <sheet name="Indeclinables" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="1114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="1144">
   <si>
     <t>upasaṃkamati</t>
   </si>
@@ -3294,12 +3295,6 @@
     <t>kāraka</t>
   </si>
   <si>
-    <t>1. paccattavacana</t>
-  </si>
-  <si>
-    <t>2. upayogavacana</t>
-  </si>
-  <si>
     <t>ahaṃ</t>
   </si>
   <si>
@@ -3336,18 +3331,9 @@
     <t>tā</t>
   </si>
   <si>
-    <t>he</t>
-  </si>
-  <si>
-    <t>she</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>they</t>
-  </si>
-  <si>
     <t>you(s)</t>
   </si>
   <si>
@@ -3357,31 +3343,136 @@
     <t>you (thou)</t>
   </si>
   <si>
-    <t>him/her</t>
-  </si>
-  <si>
     <t>you (thee)</t>
   </si>
   <si>
     <t>me</t>
   </si>
   <si>
-    <t>them</t>
-  </si>
-  <si>
-    <t>niyamita</t>
-  </si>
-  <si>
-    <t>rūpa</t>
-  </si>
-  <si>
     <t>tad</t>
   </si>
   <si>
-    <t>the, this</t>
-  </si>
-  <si>
     <t>tāni</t>
+  </si>
+  <si>
+    <t>the, that, it (anaphoric)</t>
+  </si>
+  <si>
+    <t>etaṃ</t>
+  </si>
+  <si>
+    <t>this, it (deictic)</t>
+  </si>
+  <si>
+    <t>etad</t>
+  </si>
+  <si>
+    <t>eso</t>
+  </si>
+  <si>
+    <t>he, this, it (deictic)</t>
+  </si>
+  <si>
+    <t>esa</t>
+  </si>
+  <si>
+    <t>she, this, it (deictic)</t>
+  </si>
+  <si>
+    <t>esā</t>
+  </si>
+  <si>
+    <t>pumitthiliṅga</t>
+  </si>
+  <si>
+    <t>him, her, the, that, it (anaphoric)</t>
+  </si>
+  <si>
+    <t>they, those  (anaphoric)</t>
+  </si>
+  <si>
+    <t>them, those  (anaphoric)</t>
+  </si>
+  <si>
+    <t>etāni</t>
+  </si>
+  <si>
+    <t>ete</t>
+  </si>
+  <si>
+    <t>etā</t>
+  </si>
+  <si>
+    <t>they, this, it (deictic)</t>
+  </si>
+  <si>
+    <t>paccattavacana</t>
+  </si>
+  <si>
+    <t>upayogavacana</t>
+  </si>
+  <si>
+    <t>he, that, it (anaphoric)</t>
+  </si>
+  <si>
+    <t>she, that, it (anaphoric)</t>
+  </si>
+  <si>
+    <t>ayaṃ</t>
+  </si>
+  <si>
+    <t>idaṃ</t>
+  </si>
+  <si>
+    <t>he, she, this, it (deictic)</t>
+  </si>
+  <si>
+    <t>imāni</t>
+  </si>
+  <si>
+    <t>they, these (deictic)</t>
+  </si>
+  <si>
+    <t>ime</t>
+  </si>
+  <si>
+    <t>imā</t>
+  </si>
+  <si>
+    <t>jāti</t>
+  </si>
+  <si>
+    <t>puggalanāma</t>
+  </si>
+  <si>
+    <t>nidassananāma</t>
+  </si>
+  <si>
+    <t>bhagavā</t>
+  </si>
+  <si>
+    <t>bhagavanto</t>
+  </si>
+  <si>
+    <t>bhagavantaṃ</t>
+  </si>
+  <si>
+    <t>brahmā</t>
+  </si>
+  <si>
+    <t>brahmāno</t>
+  </si>
+  <si>
+    <t>brahmānaṃ</t>
+  </si>
+  <si>
+    <t>rāja</t>
+  </si>
+  <si>
+    <t>rājanto</t>
+  </si>
+  <si>
+    <t>rājānaṃ</t>
   </si>
 </sst>
 </file>
@@ -3766,7 +3857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EEF752-1E38-D246-B3C3-5032ABA633EF}">
   <dimension ref="A1:K188"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9741,7 +9832,7 @@
   <dimension ref="A1:F133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C39"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12416,21 +12507,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2215B98-3D7B-2C49-9925-33FA782F49C9}">
-  <dimension ref="A1:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61F19DE-F0D9-304B-B2F1-DE9E619D03DB}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>502</v>
       </c>
@@ -12441,833 +12531,331 @@
         <v>500</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1075</v>
+        <v>1132</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1110</v>
+        <v>1076</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1076</v>
+        <v>1083</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1077</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1083</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>1075</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>499</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>1109</v>
+        <v>287</v>
       </c>
       <c r="E2" t="s">
-        <v>1089</v>
+        <v>1081</v>
       </c>
       <c r="F2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="H2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E4" t="s">
         <v>1081</v>
       </c>
-      <c r="G2" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I2" t="s">
-        <v>511</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>499</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1137</v>
+      </c>
+      <c r="H4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="H5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E6" t="s">
         <v>1081</v>
       </c>
-      <c r="G3" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I3" t="s">
-        <v>511</v>
-      </c>
-      <c r="J3" t="s">
-        <v>1111</v>
-      </c>
-      <c r="K3" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>499</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1138</v>
+      </c>
+      <c r="H6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>287</v>
+      </c>
+      <c r="E8" t="s">
         <v>1081</v>
       </c>
-      <c r="G4" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1092</v>
-      </c>
-      <c r="K4" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>499</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="F8" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H8" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>499</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1139</v>
+      </c>
+      <c r="H9" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>499</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E10" t="s">
         <v>1081</v>
       </c>
-      <c r="G5" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H5" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I5" t="s">
-        <v>94</v>
-      </c>
-      <c r="J5" t="s">
-        <v>1094</v>
-      </c>
-      <c r="K5" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>499</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="F10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1141</v>
+      </c>
+      <c r="H10" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>287</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="H11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E12" t="s">
         <v>1081</v>
       </c>
-      <c r="G6" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H6" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I6" t="s">
-        <v>690</v>
-      </c>
-      <c r="J6" t="s">
-        <v>1095</v>
-      </c>
-      <c r="K6" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>499</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I7" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J7" t="s">
-        <v>1090</v>
-      </c>
-      <c r="K7" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>499</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G8" t="s">
-        <v>1080</v>
-      </c>
-      <c r="H8" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I8" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J8" t="s">
-        <v>1086</v>
-      </c>
-      <c r="K8" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>499</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="F12" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1143</v>
+      </c>
+      <c r="H12" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>499</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>287</v>
+      </c>
+      <c r="E13" t="s">
         <v>1082</v>
       </c>
-      <c r="G9" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I9" t="s">
-        <v>511</v>
-      </c>
-      <c r="J9" t="s">
-        <v>1113</v>
-      </c>
-      <c r="K9" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>499</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G10" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I10" t="s">
-        <v>94</v>
-      </c>
-      <c r="J10" t="s">
-        <v>1096</v>
-      </c>
-      <c r="K10" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>499</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G11" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H11" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I11" t="s">
-        <v>690</v>
-      </c>
-      <c r="J11" t="s">
-        <v>1097</v>
-      </c>
-      <c r="K11" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>499</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1093</v>
-      </c>
-      <c r="K12" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>499</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E13" t="s">
-        <v>1089</v>
-      </c>
       <c r="F13" t="s">
-        <v>1082</v>
+        <v>1122</v>
       </c>
       <c r="G13" t="s">
-        <v>1080</v>
+        <v>1142</v>
       </c>
       <c r="H13" t="s">
-        <v>1084</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J13" t="s">
-        <v>1087</v>
-      </c>
-      <c r="K13" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>499</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>27</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G14" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I14" t="s">
-        <v>511</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K14" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>499</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I15" t="s">
-        <v>511</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1111</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>499</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16">
-        <v>27</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E16" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I16" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J16" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K16" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>499</v>
-      </c>
-      <c r="B17">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1090</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>499</v>
-      </c>
-      <c r="B18">
-        <v>4</v>
-      </c>
-      <c r="C18">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F18" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G18" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I18" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J18" t="s">
-        <v>1009</v>
-      </c>
-      <c r="K18" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>499</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-      <c r="C19">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F19" t="s">
-        <v>1081</v>
-      </c>
-      <c r="G19" t="s">
-        <v>1080</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I19" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J19" t="s">
-        <v>1088</v>
-      </c>
-      <c r="K19" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>499</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>27</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G20" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H20" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I20" t="s">
-        <v>511</v>
-      </c>
-      <c r="J20" t="s">
-        <v>1113</v>
-      </c>
-      <c r="K20" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>499</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G21" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H21" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I21" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" t="s">
-        <v>1096</v>
-      </c>
-      <c r="K21" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>499</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E22" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F22" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G22" t="s">
-        <v>1078</v>
-      </c>
-      <c r="H22" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I22" t="s">
-        <v>690</v>
-      </c>
-      <c r="J22" t="s">
-        <v>1097</v>
-      </c>
-      <c r="K22" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>499</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23">
-        <v>27</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E23" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G23" t="s">
-        <v>1079</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I23" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J23" t="s">
-        <v>1093</v>
-      </c>
-      <c r="K23" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>499</v>
-      </c>
-      <c r="B24">
-        <v>4</v>
-      </c>
-      <c r="C24">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1109</v>
-      </c>
-      <c r="E24" t="s">
-        <v>1089</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1082</v>
-      </c>
-      <c r="G24" t="s">
-        <v>1080</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1085</v>
-      </c>
-      <c r="I24" t="s">
-        <v>1091</v>
-      </c>
-      <c r="J24" t="s">
-        <v>1089</v>
-      </c>
-      <c r="K24" t="s">
-        <v>1103</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -13276,6 +12864,1500 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2215B98-3D7B-2C49-9925-33FA782F49C9}">
+  <dimension ref="A1:J46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="28.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1083</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1075</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>499</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H2" t="s">
+        <v>511</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>511</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1090</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1092</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H6" t="s">
+        <v>690</v>
+      </c>
+      <c r="I6" t="s">
+        <v>1093</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>499</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="J8" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>499</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H9" t="s">
+        <v>511</v>
+      </c>
+      <c r="I9" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J9" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>499</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H10" t="s">
+        <v>94</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>499</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H11" t="s">
+        <v>690</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>499</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>499</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J14" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>499</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G15" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H15" t="s">
+        <v>511</v>
+      </c>
+      <c r="I15" t="s">
+        <v>1102</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>499</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G16" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I16" t="s">
+        <v>1088</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>499</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>499</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1086</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>499</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G19" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H19" t="s">
+        <v>511</v>
+      </c>
+      <c r="I19" t="s">
+        <v>1103</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G20" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1094</v>
+      </c>
+      <c r="J20" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>499</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H21" t="s">
+        <v>690</v>
+      </c>
+      <c r="I21" t="s">
+        <v>1095</v>
+      </c>
+      <c r="J21" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>499</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>499</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1133</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1078</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1087</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>499</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>27</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H24" t="s">
+        <v>511</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1105</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>499</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H25" t="s">
+        <v>511</v>
+      </c>
+      <c r="I25" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>499</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H26" t="s">
+        <v>94</v>
+      </c>
+      <c r="I26" t="s">
+        <v>1108</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>499</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1110</v>
+      </c>
+      <c r="J27" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>499</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H28" t="s">
+        <v>690</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1112</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>499</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H29" t="s">
+        <v>511</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>499</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H30" t="s">
+        <v>94</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>499</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>27</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H31" t="s">
+        <v>690</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>499</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1105</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>499</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>27</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H33" t="s">
+        <v>511</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1107</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>499</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H34" t="s">
+        <v>511</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1117</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>499</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H35" t="s">
+        <v>94</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>499</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>27</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H36" t="s">
+        <v>690</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1119</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>499</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H37" t="s">
+        <v>511</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>499</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I38" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>499</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H39" t="s">
+        <v>511</v>
+      </c>
+      <c r="I39" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J39" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>499</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G40" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H40" t="s">
+        <v>94</v>
+      </c>
+      <c r="I40" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J40" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>499</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G41" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H41" t="s">
+        <v>690</v>
+      </c>
+      <c r="I41" t="s">
+        <v>1131</v>
+      </c>
+      <c r="J41" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>499</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>27</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G42" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H42" t="s">
+        <v>511</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1126</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>499</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>27</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G43" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H43" t="s">
+        <v>1113</v>
+      </c>
+      <c r="I43" t="s">
+        <v>1125</v>
+      </c>
+      <c r="J43" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>499</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G44" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H44" t="s">
+        <v>511</v>
+      </c>
+      <c r="I44" t="s">
+        <v>1128</v>
+      </c>
+      <c r="J44" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>499</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H45" t="s">
+        <v>94</v>
+      </c>
+      <c r="I45" t="s">
+        <v>1130</v>
+      </c>
+      <c r="J45" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>499</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>27</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1082</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="G46" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H46" t="s">
+        <v>690</v>
+      </c>
+      <c r="I46" t="s">
+        <v>1131</v>
+      </c>
+      <c r="J46" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69360A60-59EE-0441-BA88-89364E1282A8}">
   <dimension ref="A1:E28"/>
   <sheetViews>
@@ -13769,7 +14851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{942D2CA4-63A6-ED48-9FE6-C697C2E3C617}">
   <dimension ref="A1:E52"/>
   <sheetViews>

</xml_diff>